<commit_message>
arreglo vista de creacion
</commit_message>
<xml_diff>
--- a/data base/onAirCampos.xlsx
+++ b/data base/onAirCampos.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,14 +17,14 @@
     <sheet name="listados" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$144</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$147</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1789" uniqueCount="900">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1791" uniqueCount="900">
   <si>
     <t>fuente</t>
   </si>
@@ -2729,7 +2729,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2930,23 +2930,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2982,23 +2965,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3174,12 +3140,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L147"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D121" sqref="D121"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J104" sqref="J104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4739,6 +4705,9 @@
       <c r="H53" s="5" t="s">
         <v>126</v>
       </c>
+      <c r="J53" s="5" t="s">
+        <v>858</v>
+      </c>
       <c r="L53" s="5" t="s">
         <v>887</v>
       </c>
@@ -4759,6 +4728,9 @@
       <c r="H54" s="5" t="s">
         <v>126</v>
       </c>
+      <c r="J54" s="5" t="s">
+        <v>858</v>
+      </c>
       <c r="L54" s="5" t="s">
         <v>886</v>
       </c>
@@ -7005,14 +6977,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I144" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I147"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7035,7 +7007,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P74"/>
   <sheetViews>
     <sheetView topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">

</xml_diff>